<commit_message>
added spec details view on project details page
</commit_message>
<xml_diff>
--- a/Final_Project_Table_Data.xlsx
+++ b/Final_Project_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/GD/Coding/codefellows/401/final-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C257F21-797A-8B47-8DBB-2480B39CF4CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D4E0F2-1ECE-2542-9FBD-3917C254E4C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="7" xr2:uid="{F88FDB1C-3FF9-4905-B676-5439EA0E3782}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{F88FDB1C-3FF9-4905-B676-5439EA0E3782}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t>Material</t>
+  </si>
+  <si>
+    <t>3/4 Prefinished Maple Plywood</t>
+  </si>
+  <si>
+    <t>3/4 A1 Select Maple Plywood</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1713,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2161,10 +2167,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E3F15D-9C5E-4766-9CBB-C156829E4256}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2332,10 +2338,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="C7">
         <v>0.75</v>
@@ -2347,7 +2353,7 @@
         <v>96</v>
       </c>
       <c r="F7">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="G7">
         <v>0.15</v>
@@ -2358,10 +2364,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="C8">
         <v>0.75</v>
@@ -2373,7 +2379,7 @@
         <v>96</v>
       </c>
       <c r="F8">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="G8">
         <v>0.15</v>
@@ -2384,25 +2390,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <v>0.75</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E9">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="F9">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="G9">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H9">
         <v>0.2</v>
@@ -2410,10 +2416,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C10">
         <v>0.75</v>
@@ -2425,7 +2431,7 @@
         <v>120</v>
       </c>
       <c r="F10">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10">
         <v>0.1</v>
@@ -2436,10 +2442,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11">
         <v>0.75</v>
@@ -2462,10 +2468,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12">
         <v>0.75</v>
@@ -2488,10 +2494,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13">
         <v>0.75</v>
@@ -2503,7 +2509,7 @@
         <v>120</v>
       </c>
       <c r="F13">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="G13">
         <v>0.1</v>
@@ -2514,10 +2520,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14">
         <v>0.75</v>
@@ -2540,10 +2546,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15">
         <v>0.75</v>
@@ -2566,10 +2572,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16">
         <v>0.75</v>
@@ -2592,22 +2598,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C17">
         <v>0.75</v>
       </c>
       <c r="D17">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E17">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="F17">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="G17">
         <v>0.1</v>
@@ -2618,10 +2624,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18">
         <v>0.75</v>
@@ -2633,7 +2639,7 @@
         <v>96</v>
       </c>
       <c r="F18">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>0.1</v>
@@ -2644,10 +2650,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="C19">
         <v>0.75</v>
@@ -2659,7 +2665,7 @@
         <v>96</v>
       </c>
       <c r="F19">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G19">
         <v>0.1</v>
@@ -2670,13 +2676,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D20">
         <v>48</v>
@@ -2688,9 +2694,61 @@
         <v>40</v>
       </c>
       <c r="G20">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
         <v>0.2</v>
       </c>
-      <c r="H20">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C21">
+        <v>0.75</v>
+      </c>
+      <c r="D21">
+        <v>48</v>
+      </c>
+      <c r="E21">
+        <v>96</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>48</v>
+      </c>
+      <c r="E22">
+        <v>96</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
+      </c>
+      <c r="G22">
+        <v>0.2</v>
+      </c>
+      <c r="H22">
         <v>0.2</v>
       </c>
     </row>
@@ -2778,7 +2836,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -5818,7 +5876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B892EEE5-FE5E-7440-BEA9-3A69116FAA13}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>